<commit_message>
fix bug in import/export
</commit_message>
<xml_diff>
--- a/proposals/ProposalsAfterProcess.xlsx
+++ b/proposals/ProposalsAfterProcess.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fanyang2/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fanyang2/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17600" tabRatio="500"/>
+    <workbookView xWindow="8900" yWindow="4980" windowWidth="28800" windowHeight="17600" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,9 +27,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
-    <t>test</t>
+    <t>3rqwe</t>
+  </si>
+  <si>
+    <t>eqwrewq</t>
   </si>
 </sst>
 </file>
@@ -344,22 +347,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B6:B7"/>
+  <dimension ref="F3:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="6" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B6" t="s">
+    <row r="3" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B7">
-        <v>1231</v>
+    <row r="4" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F4" t="s">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
implement final proposal import without test
</commit_message>
<xml_diff>
--- a/proposals/ProposalsAfterProcess.xlsx
+++ b/proposals/ProposalsAfterProcess.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28908"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="28908"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fanyang2/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fanyang2/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="8900" yWindow="4980" windowWidth="28800" windowHeight="17600" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="5180" windowWidth="45880" windowHeight="22020"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="144525" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -27,25 +27,93 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
-  <si>
-    <t>3rqwe</t>
-  </si>
-  <si>
-    <t>eqwrewq</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+  <si>
+    <t>proposal_id</t>
+  </si>
+  <si>
+    <t>proposal_title</t>
+  </si>
+  <si>
+    <t>project_location</t>
+  </si>
+  <si>
+    <t>cost</t>
+  </si>
+  <si>
+    <t>proposal_idea</t>
+  </si>
+  <si>
+    <t>proposal_need</t>
+  </si>
+  <si>
+    <t>proposal_latitude</t>
+  </si>
+  <si>
+    <t>proposal_longitude</t>
+  </si>
+  <si>
+    <t>project_type</t>
+  </si>
+  <si>
+    <t>department</t>
+  </si>
+  <si>
+    <t>who_benefits</t>
+  </si>
+  <si>
+    <t>council_district</t>
+  </si>
+  <si>
+    <t>neihborhood</t>
+  </si>
+  <si>
+    <t>Waterpump7</t>
+  </si>
+  <si>
+    <t>9rd Ave, Belltown</t>
+  </si>
+  <si>
+    <t>build a lot water pumps for fire fighter</t>
+  </si>
+  <si>
+    <t>firefighter</t>
+  </si>
+  <si>
+    <t>security</t>
+  </si>
+  <si>
+    <t>SHE</t>
+  </si>
+  <si>
+    <t>everyone</t>
+  </si>
+  <si>
+    <t>belltown</t>
+  </si>
+  <si>
+    <t>20180506073000</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
-      <sz val="12"/>
-      <color theme="1"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -65,13 +133,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+  <cellStyleXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+  <cellXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyProtection="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyProtection="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -95,39 +166,39 @@
         <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="44546A"/>
+        <a:srgbClr val="1F497D"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="E7E6E6"/>
+        <a:srgbClr val="EEECE1"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="4F81BD"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="ED7D31"/>
+        <a:srgbClr val="C0504D"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="A5A5A5"/>
+        <a:srgbClr val="9BBB59"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="FFC000"/>
+        <a:srgbClr val="8064A2"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="4BACC6"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="70AD47"/>
+        <a:srgbClr val="F79646"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0563C1"/>
+        <a:srgbClr val="0000FF"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="954F72"/>
+        <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="Yu Gothic Light"/>
@@ -206,166 +277,277 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:lumMod val="110000"/>
-                <a:satMod val="105000"/>
-                <a:tint val="67000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="103000"/>
-                <a:tint val="73000"/>
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="109000"/>
-                <a:tint val="81000"/>
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:satMod val="103000"/>
-                <a:lumMod val="102000"/>
-                <a:tint val="94000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:satMod val="110000"/>
-                <a:lumMod val="100000"/>
-                <a:shade val="100000"/>
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="99000"/>
-                <a:satMod val="120000"/>
-                <a:shade val="78000"/>
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="16200000" scaled="0"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
         </a:ln>
       </a:lnStyleLst>
       <a:effectStyleLst>
         <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
-                <a:alpha val="63000"/>
+                <a:alpha val="35000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
       <a:bgFillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:tint val="95000"/>
-            <a:satMod val="170000"/>
-          </a:schemeClr>
-        </a:solidFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="93000"/>
-                <a:satMod val="150000"/>
-                <a:shade val="98000"/>
-                <a:lumMod val="102000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:tint val="98000"/>
-                <a:satMod val="130000"/>
-                <a:shade val="90000"/>
-                <a:lumMod val="103000"/>
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="63000"/>
-                <a:satMod val="120000"/>
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
   <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="F3:F4"/>
+  <dimension ref="A1:M2"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView tabSelected="1" zoomScale="176" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.1640625" customWidth="1"/>
+    <col min="5" max="5" width="29.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.83203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="3" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F3" t="s">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="4" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F4" t="s">
-        <v>1</v>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2">
+        <v>60</v>
+      </c>
+      <c r="E2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2">
+        <v>47.662199999999999</v>
+      </c>
+      <c r="H2">
+        <v>-122.3721</v>
+      </c>
+      <c r="I2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J2" t="s">
+        <v>18</v>
+      </c>
+      <c r="K2" t="s">
+        <v>19</v>
+      </c>
+      <c r="L2">
+        <v>3</v>
+      </c>
+      <c r="M2" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
 </worksheet>
 </file>
</xml_diff>